<commit_message>
added various new Profiles. No Instances Yet. Not added to Composition yet.
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-pathologic-side.xlsx
+++ b/docs/StructureDefinition-pathologic-side.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-05-07T21:31:29+02:00</t>
+    <t>2025-05-12T20:06:16+02:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -69,7 +69,7 @@
     <t>Contact</t>
   </si>
   <si>
-    <t>Constantin Renner (https://github.com/cdeveHealth, constantinrenner1@gmail.com)</t>
+    <t>Constantin Renner (http://example.org/example-publisher, constantinrenner1@gmail.com)</t>
   </si>
   <si>
     <t>Jurisdiction</t>

</xml_diff>

<commit_message>
correct reference added to examples.
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-pathologic-side.xlsx
+++ b/docs/StructureDefinition-pathologic-side.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-05-12T20:06:16+02:00</t>
+    <t>2025-05-13T19:16:00+02:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -69,7 +69,7 @@
     <t>Contact</t>
   </si>
   <si>
-    <t>Constantin Renner (http://example.org/example-publisher, constantinrenner1@gmail.com)</t>
+    <t>Constantin Renner (https://github.com/cdeveHealth, constantinrenner1@gmail.com)</t>
   </si>
   <si>
     <t>Jurisdiction</t>

</xml_diff>

<commit_message>
Deploy latest IG. Borken Links fixed.
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-pathologic-side.xlsx
+++ b/docs/StructureDefinition-pathologic-side.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-05-14T23:43:24+02:00</t>
+    <t>2025-05-19T18:20:06+02:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -69,7 +69,7 @@
     <t>Contact</t>
   </si>
   <si>
-    <t>Constantin Renner (https://github.com/cdeveHealth, constantinrenner1@gmail.com)</t>
+    <t>Constantin Renner (https://github.com/medinterop-renner/TraumaIG, constantinrenner1@gmail.com)</t>
   </si>
   <si>
     <t>Jurisdiction</t>

</xml_diff>